<commit_message>
Added Allure reporting, updated pom.xml and workflow
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17070" windowHeight="3375" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17040" windowHeight="2745" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
     <sheet name="Products" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:Q9"/>
+  <oleSize ref="A1:Q4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -56,13 +56,13 @@
     <t>ExpectedResult</t>
   </si>
   <si>
-    <t>iPhone 15</t>
-  </si>
-  <si>
-    <t>Samsung S24</t>
-  </si>
-  <si>
     <t>Pixel 9</t>
+  </si>
+  <si>
+    <t>iPhone</t>
+  </si>
+  <si>
+    <t>Palm Treo Pro</t>
   </si>
 </sst>
 </file>
@@ -482,10 +482,13 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
@@ -495,17 +498,17 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>12</v>
+    <row r="3" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
       </c>
       <c r="B3" s="3" t="b">
         <v>1</v>
@@ -513,13 +516,14 @@
     </row>
     <row r="4" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>